<commit_message>
Commiting changes to plan sheet
</commit_message>
<xml_diff>
--- a/results/Prediction_RMSE_comparison.xlsx
+++ b/results/Prediction_RMSE_comparison.xlsx
@@ -19,7 +19,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="B2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -27,7 +27,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t>Author:</t>
         </r>
@@ -36,10 +36,10 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
-Time consuming and difficult to handle multiple features</t>
+Adjusted after using actual unemployment rate</t>
         </r>
       </text>
     </comment>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Canada</t>
   </si>
@@ -83,31 +83,23 @@
     <t>Univariate using Prophet</t>
   </si>
   <si>
-    <t>Shresth</t>
-  </si>
-  <si>
     <t>Ankit</t>
   </si>
   <si>
-    <t>Pradeep</t>
+    <t>Shresth/Pradeep</t>
+  </si>
+  <si>
+    <t>Ankit/Pradeep</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -124,17 +116,17 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,12 +136,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -194,13 +180,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,7 +493,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -528,7 +513,7 @@
       <c r="C1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -540,27 +525,27 @@
         <v>5</v>
       </c>
       <c r="B2">
-        <v>9.3299999999999994E-2</v>
+        <v>0.10808</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2">
         <v>0.11700000000000001</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>0.13956399999999999</v>
+      </c>
+      <c r="C3" t="s">
         <v>13</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
       </c>
       <c r="E3">
         <v>9.8299999999999998E-2</v>
@@ -570,31 +555,43 @@
       <c r="A4" s="3" t="s">
         <v>0</v>
       </c>
+      <c r="B4">
+        <v>0.16039700000000001</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
+      <c r="B5">
+        <v>8.4220000000000003E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
+      <c r="B6">
+        <v>0.111939</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7">
-        <v>0.14000000000000001</v>
+        <v>6.1232799999999997E-2</v>
       </c>
       <c r="C7">
-        <v>7.0000000000000007E-2</v>
+        <v>7.6999999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7.9339800000000002E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor fix results doc
</commit_message>
<xml_diff>
--- a/results/Prediction_RMSE_comparison.xlsx
+++ b/results/Prediction_RMSE_comparison.xlsx
@@ -17,19 +17,6 @@
     </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author> </author>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0">
-      <text/>
-    </comment>
-  </commentList>
-</comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -220,7 +207,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
lstm can fra ger
</commit_message>
<xml_diff>
--- a/results/Prediction_RMSE_comparison.xlsx
+++ b/results/Prediction_RMSE_comparison.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="23">
   <si>
     <t xml:space="preserve">Country</t>
   </si>
@@ -56,9 +56,6 @@
   </si>
   <si>
     <t xml:space="preserve">France</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ankit/Pradeep</t>
   </si>
   <si>
     <t xml:space="preserve">Germany</t>
@@ -267,7 +264,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="18">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -307,14 +304,28 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFA3DF13"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFB700"/>
+          <fgColor rgb="FF94DA17"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF89D619"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8BD718"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E60F"/>
         </patternFill>
       </fill>
     </dxf>
@@ -335,21 +346,14 @@
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <fgColor rgb="FFFFB400"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF83D41A"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFA6E013"/>
+          <fgColor rgb="FFFF9100"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFD00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -357,6 +361,34 @@
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FFD5F009"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFE2F506"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC200"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFCA00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8DD818"/>
         </patternFill>
       </fill>
     </dxf>
@@ -376,7 +408,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -420,6 +452,9 @@
       <c r="B2" s="1" t="n">
         <v>0.160397</v>
       </c>
+      <c r="C2" s="1" t="n">
+        <v>0.222352</v>
+      </c>
       <c r="E2" s="5" t="n">
         <v>1.850288</v>
       </c>
@@ -434,8 +469,8 @@
       <c r="B3" s="1" t="n">
         <v>0.139564</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>9</v>
+      <c r="C3" s="1" t="n">
+        <v>0.22929</v>
       </c>
       <c r="D3" s="1" t="n">
         <v>0.70349</v>
@@ -449,11 +484,14 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>0.08422</v>
       </c>
+      <c r="C4" s="1" t="n">
+        <v>0.230484</v>
+      </c>
       <c r="E4" s="5" t="n">
         <v>0.07215</v>
       </c>
@@ -463,7 +501,7 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0.111939</v>
@@ -477,7 +515,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>0.0612328</v>
@@ -494,13 +532,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>0.10808</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="5" t="n">
         <v>0.285329</v>
@@ -514,7 +552,7 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0.0793398</v>
@@ -653,19 +691,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -682,7 +720,7 @@
         <v>6.04784</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1.9688</v>
@@ -702,7 +740,7 @@
         <v>6.729585</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>0.0983</v>
@@ -710,7 +748,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="8" t="n">
         <v>3.1088488</v>
@@ -722,7 +760,7 @@
         <v>2.851482</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>0.1846</v>
@@ -730,7 +768,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8" t="n">
         <v>8.14796</v>
@@ -742,7 +780,7 @@
         <v>7.817619</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>0.4779</v>
@@ -750,7 +788,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="8" t="n">
         <v>2.008909</v>
@@ -762,7 +800,7 @@
         <v>2.013057</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>0.4308</v>
@@ -770,7 +808,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="8" t="n">
         <v>3.385219</v>
@@ -782,7 +820,7 @@
         <v>2.973279</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>0.1765</v>
@@ -790,7 +828,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="8" t="n">
         <v>4.166677</v>
@@ -802,7 +840,7 @@
         <v>2.856417</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>0.737</v>
@@ -837,19 +875,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,7 +904,7 @@
         <v>8.514531</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>1.850288</v>
@@ -886,7 +924,7 @@
         <v>7.874131</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>0.258843</v>
@@ -894,7 +932,7 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="n">
         <v>2.914958</v>
@@ -906,7 +944,7 @@
         <v>2.542403</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>0.07215</v>
@@ -914,7 +952,7 @@
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>8.31146</v>
@@ -926,7 +964,7 @@
         <v>7.776296</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>0.603992</v>
@@ -934,7 +972,7 @@
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>2.212238</v>
@@ -946,7 +984,7 @@
         <v>1.782431</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>0.249625</v>
@@ -954,7 +992,7 @@
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>3.202596</v>
@@ -966,7 +1004,7 @@
         <v>1.992653</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>0.285329</v>
@@ -974,7 +1012,7 @@
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>5.522781</v>
@@ -986,7 +1024,7 @@
         <v>7.392238</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>2.035041</v>
@@ -1021,19 +1059,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,7 +1079,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1049,7 +1087,7 @@
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="9" t="n">
         <v>0.70349</v>
@@ -1057,42 +1095,42 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1124,19 +1162,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1144,7 +1182,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1152,47 +1190,47 @@
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1224,19 +1262,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1244,7 +1282,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1252,47 +1290,47 @@
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -1324,19 +1362,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>19</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1344,7 +1382,7 @@
         <v>7</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,47 +1390,47 @@
         <v>8</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>